<commit_message>
Release 0.3.4 CW3M_McKenzie.envx - Remove an obsolete comment. Flow_McKenzie.xml - Add observations to "FLOW McKenzie daily outflows at gages (cfs)". CW3M_McKenzie_Script.iss - Change release number to 0.3.4. envmsg.cpp - Comment out the duplicative call to AfxGetMainWnd()->MessageBox(). Flow.cpp - Warn the user if the calendar for the observations is different from the calendar for the simulation.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3Mhandbook.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3Mhandbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA6689-66EA-4F28-9F8C-E987C9ED20F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51269D1D-0057-46C1-B50E-683918D34DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2295" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="2" xr2:uid="{6F1FA268-D9FD-4F4F-A15F-38D57FB8B652}"/>
+    <workbookView xWindow="-25080" yWindow="-105" windowWidth="24030" windowHeight="13050" activeTab="2" xr2:uid="{6F1FA268-D9FD-4F4F-A15F-38D57FB8B652}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Areas" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="206">
   <si>
     <t>Marys</t>
   </si>
@@ -1191,6 +1191,9 @@
   </si>
   <si>
     <t>Oak Creek</t>
+  </si>
+  <si>
+    <t>Upper Willamette mainstem</t>
   </si>
 </sst>
 </file>
@@ -2927,8 +2930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAC400F-E210-4250-95F2-221A12BB9102}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,7 +3320,7 @@
         <v>16</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>46</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>